<commit_message>
WIP - Bug Fixing_2
</commit_message>
<xml_diff>
--- a/UpdateDependencies_Log.xlsx
+++ b/UpdateDependencies_Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\randomly-read\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AEF936-92B8-4272-BAEF-EA14B42413E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545ADAC2-A671-4485-8C07-0B020EE66C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18195" yWindow="0" windowWidth="18300" windowHeight="15585" activeTab="1" xr2:uid="{3C2A457F-0F99-4D56-BC5D-761AB251847F}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{3C2A457F-0F99-4D56-BC5D-761AB251847F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -649,7 +649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -658,11 +658,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1015,7 +1011,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1023,7 +1019,7 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1082,7 +1078,7 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>121</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1301,7 +1297,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D36" t="s">
@@ -1463,7 +1459,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="6" t="s">
+      <c r="A51" t="s">
         <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -1510,7 +1506,7 @@
       <c r="A55" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="6" t="s">
         <v>133</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -1607,8 +1603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F54773C-8EDC-4C1E-9F26-CF639F77861D}">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1903,7 +1899,7 @@
       <c r="A37" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2038,7 +2034,7 @@
       <c r="A55" t="s">
         <v>49</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>